<commit_message>
fix DNA and RNA stoi
Here I fix the stoichiometry of the DNA and RNA metabolites in the Biomass equation based on calculations made in the Biomass_rct.xlsx file.
</commit_message>
<xml_diff>
--- a/databases/Biomass_rct.xlsx
+++ b/databases/Biomass_rct.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="162">
   <si>
     <t>Biomass reaction</t>
   </si>
@@ -497,6 +497,21 @@
   </si>
   <si>
     <t>-0.102432476287413</t>
+  </si>
+  <si>
+    <t>GC content</t>
+  </si>
+  <si>
+    <t>This is way too high, so I don't trust this. I will use the estimation above.</t>
+  </si>
+  <si>
+    <t>Use estimation from GC content</t>
+  </si>
+  <si>
+    <t>-0.00867142964560465</t>
+  </si>
+  <si>
+    <t>-0.00664911743143537</t>
   </si>
 </sst>
 </file>
@@ -504,9 +519,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.0000000"/>
-    <numFmt numFmtId="173" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -531,7 +546,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,6 +571,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -569,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -581,12 +602,13 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -869,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,7 +971,9 @@
       <c r="C6" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="17" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1040,7 +1064,13 @@
       <c r="C14" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D14" s="5"/>
+      <c r="D14" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E14">
+        <f>C14-B14</f>
+        <v>-2.2435461287413E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1062,55 +1092,63 @@
       </c>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
       <c r="B17">
         <v>-2.9903042000000001E-2</v>
       </c>
-      <c r="C17" s="16">
-        <v>-2.2928567250000004E-2</v>
-      </c>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18">
         <v>-2.3333636000000001E-2</v>
       </c>
-      <c r="C18" s="16">
-        <v>-7.0392066000000003E-2</v>
-      </c>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
       <c r="B19">
         <v>-2.3333636000000001E-2</v>
       </c>
-      <c r="C19" s="16">
-        <v>-7.0392066000000003E-2</v>
-      </c>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
       <c r="B20">
         <v>-2.9903042000000001E-2</v>
       </c>
-      <c r="C20" s="16">
-        <v>-2.2928567250000004E-2</v>
-      </c>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1118,7 +1156,7 @@
         <v>-2.9903042000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1130,7 +1168,7 @@
       </c>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1142,7 +1180,7 @@
       </c>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1154,7 +1192,7 @@
       </c>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1166,7 +1204,7 @@
       </c>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1178,7 +1216,7 @@
       </c>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1188,9 +1226,15 @@
       <c r="C27" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27">
+        <f>C27-B27</f>
+        <v>4.3519523712586994E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1198,7 +1242,7 @@
         <v>-2.9903042000000001E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -1209,7 +1253,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1220,7 +1264,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1232,7 +1276,7 @@
       </c>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1464,7 +1508,9 @@
       <c r="C52" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D52" s="5"/>
+      <c r="D52" s="17" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -1599,10 +1645,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" activeCellId="1" sqref="E20:E23 A20:A23"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1613,7 +1659,7 @@
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>116</v>
       </c>
@@ -1637,7 +1683,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>129</v>
       </c>
@@ -1648,7 +1694,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>113</v>
       </c>
@@ -1666,7 +1712,7 @@
         <v>8.6714296456046544E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -1685,7 +1731,7 @@
         <v>8.6714296456046544E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -1707,7 +1753,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -1726,7 +1772,7 @@
         <v>8.6714296456046544E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -1745,18 +1791,18 @@
         <v>6.6491174314353696E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D8" s="15">
         <f>SUM(D4:D7)</f>
         <v>326.35910290000004</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>139</v>
       </c>
@@ -1781,8 +1827,15 @@
       <c r="I10" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="K10">
+        <f>J12*2</f>
+        <v>75.430334695033793</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -1810,8 +1863,12 @@
         <f>AVERAGE(B11:E11)</f>
         <v>2.2928567250000004E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="16">
+        <f>100*I11/$I$15</f>
+        <v>12.2848326524831</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -1839,8 +1896,12 @@
         <f t="shared" ref="I12:I14" si="4">AVERAGE(B12:E12)</f>
         <v>7.0392066000000003E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="16">
+        <f t="shared" ref="J12:J13" si="5">100*I12/$I$15</f>
+        <v>37.715167347516896</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -1868,8 +1929,12 @@
         <f t="shared" si="4"/>
         <v>2.2928567250000004E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="16">
+        <f t="shared" si="5"/>
+        <v>12.2848326524831</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -1897,8 +1962,21 @@
         <f t="shared" si="4"/>
         <v>7.0392066000000003E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="16">
+        <f>100*I14/$I$15</f>
+        <v>37.715167347516896</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <f>SUM(I11:I14)</f>
+        <v>0.18664126650000001</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>121</v>
       </c>
@@ -1976,11 +2054,11 @@
         <v>21.7</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D23" si="5">B21*C21/100</f>
+        <f t="shared" ref="D21:D23" si="6">B21*C21/100</f>
         <v>70.134399999999999</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:E23" si="6">(C21/100)*$G$16*1000</f>
+        <f t="shared" ref="E21:E23" si="7">(C21/100)*$G$16*1000</f>
         <v>0.10243247628741278</v>
       </c>
     </row>
@@ -1995,11 +2073,11 @@
         <v>28.3</v>
       </c>
       <c r="D22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>91.74860000000001</v>
       </c>
       <c r="E22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.13358705432874571</v>
       </c>
     </row>
@@ -2014,11 +2092,11 @@
         <v>21.7</v>
       </c>
       <c r="D23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>78.814399999999992</v>
       </c>
       <c r="E23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.10243247628741278</v>
       </c>
     </row>
@@ -2169,7 +2247,7 @@
         <v>180.16</v>
       </c>
       <c r="D8" s="11">
-        <f t="shared" ref="D5:D10" si="1">($D$1*B8)/100</f>
+        <f t="shared" ref="D8" si="1">($D$1*B8)/100</f>
         <v>1.1549357160000001E-3</v>
       </c>
       <c r="E8" s="12">

</xml_diff>

<commit_message>
fix other mets in rct
Here i fixed the stoichiometries of the other metabolites that were in the biomass reaction and added the 10fthf_c metabolite, according to Beata's data.
</commit_message>
<xml_diff>
--- a/databases/Biomass_rct.xlsx
+++ b/databases/Biomass_rct.xlsx
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
-    <sheet name="Cofactors" sheetId="4" r:id="rId2"/>
-    <sheet name="DNARNA" sheetId="2" r:id="rId3"/>
-    <sheet name="Carbohydrates" sheetId="3" r:id="rId4"/>
+    <sheet name="Other" sheetId="5" r:id="rId2"/>
+    <sheet name="Cofactors" sheetId="4" r:id="rId3"/>
+    <sheet name="DNARNA" sheetId="2" r:id="rId4"/>
+    <sheet name="Carbohydrates" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="189">
   <si>
     <t>Biomass reaction</t>
   </si>
@@ -561,6 +562,39 @@
   </si>
   <si>
     <t>-0.000168</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>accoa</t>
+  </si>
+  <si>
+    <t>succoa</t>
+  </si>
+  <si>
+    <t>chor</t>
+  </si>
+  <si>
+    <t>thmpp</t>
+  </si>
+  <si>
+    <t>gthrd</t>
+  </si>
+  <si>
+    <t>ptrc</t>
+  </si>
+  <si>
+    <t>B. subtilis</t>
+  </si>
+  <si>
+    <t>-0.000279</t>
+  </si>
+  <si>
+    <t>remove alltogether?</t>
+  </si>
+  <si>
+    <t>-0.03327</t>
   </si>
 </sst>
 </file>
@@ -595,7 +629,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -626,6 +660,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -639,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -659,6 +699,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -941,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,6 +1020,10 @@
       <c r="B3">
         <v>-2.9903042000000001E-2</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="4"/>
       <c r="F3" s="4" t="s">
         <v>95</v>
       </c>
@@ -1091,6 +1137,10 @@
       <c r="B12">
         <v>-2.9903042000000001E-2</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1291,6 +1341,12 @@
       <c r="B28">
         <v>-2.9903042000000001E-2</v>
       </c>
+      <c r="C28" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -1467,6 +1523,10 @@
       <c r="B43">
         <v>-2.9903042000000001E-2</v>
       </c>
+      <c r="C43" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
@@ -1511,6 +1571,10 @@
       <c r="B47">
         <v>-2.9903042000000001E-2</v>
       </c>
+      <c r="C47" s="18">
+        <v>9.7999999999999997E-5</v>
+      </c>
+      <c r="D47" s="20"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -1519,6 +1583,10 @@
       <c r="B48">
         <v>-2.9903042000000001E-2</v>
       </c>
+      <c r="C48">
+        <v>2.23E-4</v>
+      </c>
+      <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
@@ -1636,7 +1704,7 @@
       <c r="C59">
         <v>-4.0000000000000002E-4</v>
       </c>
-      <c r="D59" s="5"/>
+      <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
@@ -1702,6 +1770,95 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>2.23E-4</v>
+      </c>
+      <c r="C2">
+        <v>3.6699999999999998E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3">
+        <v>2.7900000000000001E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4">
+        <v>2.23E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5">
+        <v>2.23E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6">
+        <v>3.3270000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="18">
+        <v>9.7999999999999997E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8">
+        <v>2.23E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:A8">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -1856,7 +2013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
@@ -2325,7 +2482,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fix thmpp and succoa stoich
</commit_message>
<xml_diff>
--- a/databases/Biomass_rct.xlsx
+++ b/databases/Biomass_rct.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="190">
   <si>
     <t>Biomass reaction</t>
   </si>
@@ -595,6 +595,9 @@
   </si>
   <si>
     <t>-0.03327</t>
+  </si>
+  <si>
+    <t>-0.000098</t>
   </si>
 </sst>
 </file>
@@ -679,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -701,6 +704,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1394,7 +1398,7 @@
       </c>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1406,7 +1410,7 @@
       </c>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1418,7 +1422,7 @@
       </c>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -1430,7 +1434,7 @@
       </c>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1442,7 +1446,7 @@
       </c>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1454,7 +1458,7 @@
       </c>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1466,7 +1470,7 @@
       </c>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1478,7 +1482,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -1490,7 +1494,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -1504,7 +1508,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -1516,7 +1520,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -1528,7 +1532,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1540,7 +1544,7 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -1552,7 +1556,7 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -1564,29 +1568,32 @@
       </c>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>17</v>
       </c>
       <c r="B47">
         <v>-2.9903042000000001E-2</v>
       </c>
-      <c r="C47" s="18">
-        <v>9.7999999999999997E-5</v>
+      <c r="C47" s="21" t="s">
+        <v>189</v>
       </c>
       <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>45</v>
       </c>
       <c r="B48">
         <v>-2.9903042000000001E-2</v>
       </c>
-      <c r="C48">
-        <v>2.23E-4</v>
+      <c r="C48" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="D48" s="4"/>
+      <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">

</xml_diff>